<commit_message>
added tests results for pinsearch and superset search
</commit_message>
<xml_diff>
--- a/results/test_results.xlsx
+++ b/results/test_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\david\Documenti\PyCharmProject\hypfs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\david\Documenti\PyCharmProject\hypfs\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5720F38-D3C8-4AD4-B259-F0BF0EB6B792}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C914A9B0-C62B-4665-8285-403597602DC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pin" sheetId="1" r:id="rId1"/>
@@ -178,7 +178,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="it-IT"/>
-              <a:t>SUPERSET</a:t>
+              <a:t>SUPERSET SEARCH</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -794,7 +794,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="it-IT"/>
-              <a:t>PINSEARCH</a:t>
+              <a:t>PIN SEARCH</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2841,7 +2841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
@@ -3064,8 +3064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9153A23-4012-455E-B92D-83C7047126C1}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U31" sqref="U31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>